<commit_message>
Update Sample form - Format symbol field plug-in.xlsx
</commit_message>
<xml_diff>
--- a/extras/sample-form/Sample form - Format symbol field plug-in.xlsx
+++ b/extras/sample-form/Sample form - Format symbol field plug-in.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amrikcooper/Documents/GitHub/format-symbol/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE07D77C-991E-6E4A-9DD7-754D62F644DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607D53FD-96F4-934C-B550-A3B427A0B1ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2680,22 +2680,22 @@
     <t>intro_note</t>
   </si>
   <si>
-    <t>This is a sample form for the format-symbol field plug-in</t>
-  </si>
-  <si>
     <t>intro</t>
   </si>
   <si>
-    <t>See the dollar sign on the left of the input box.</t>
-  </si>
-  <si>
-    <t>See the percentage sign on the rihght of the input box.</t>
-  </si>
-  <si>
     <t>Sample form - Format symbol field plug-in</t>
   </si>
   <si>
     <t>sample_format_symbol</t>
+  </si>
+  <si>
+    <t>See the percentage sign on the right of the input box.</t>
+  </si>
+  <si>
+    <t>See the Dollar sign on the left of the input box.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welcome to this SurveyCTO sample form! This is a sample form for the &lt;a href="Welcome%20to this SurveyCTO sample form! This is a sample form for the format-symbol field plug-in." target="_blank" rel="noopener"&gt;format-symbol field plug-in&lt;/a&gt;.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -4696,11 +4696,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -5095,12 +5095,20 @@
       <c r="Z10" s="9"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
+      <c r="A11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>373</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>368</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -5124,23 +5132,25 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>367</v>
+        <v>39</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="D12" s="8"/>
+        <v>40</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>372</v>
+      </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>369</v>
+        <v>41</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
@@ -5163,17 +5173,17 @@
         <v>38</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="8"/>
@@ -5197,22 +5207,12 @@
       <c r="Z13" s="9"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>371</v>
-      </c>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="8"/>
       <c r="I14" s="6"/>
@@ -11002,34 +11002,7 @@
       <c r="Y220" s="9"/>
       <c r="Z220" s="9"/>
     </row>
-    <row r="221" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A221" s="6"/>
-      <c r="B221" s="6"/>
-      <c r="C221" s="7"/>
-      <c r="D221" s="8"/>
-      <c r="E221" s="6"/>
-      <c r="F221" s="6"/>
-      <c r="G221" s="6"/>
-      <c r="H221" s="8"/>
-      <c r="I221" s="6"/>
-      <c r="J221" s="6"/>
-      <c r="K221" s="6"/>
-      <c r="L221" s="6"/>
-      <c r="M221" s="6"/>
-      <c r="N221" s="6"/>
-      <c r="O221" s="6"/>
-      <c r="P221" s="6"/>
-      <c r="Q221" s="6"/>
-      <c r="R221" s="6"/>
-      <c r="S221" s="6"/>
-      <c r="T221" s="6"/>
-      <c r="U221" s="6"/>
-      <c r="V221" s="6"/>
-      <c r="W221" s="6"/>
-      <c r="X221" s="9"/>
-      <c r="Y221" s="9"/>
-      <c r="Z221" s="9"/>
-    </row>
+    <row r="221" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="222" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="223" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="224" spans="1:26" ht="15.75" customHeight="1"/>
@@ -11809,376 +11782,375 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="B1:C13 I1:I13 F1:F13 F15:F1001 I15:I1001 B15:C1001">
+  <conditionalFormatting sqref="F14:F1000 I14:I1000 B14:C1000 B1:C12 I1:I12 F1:F12">
     <cfRule type="expression" dxfId="171" priority="1" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C13 O1:O13 I1:I13 I15:I1001 O15:O1001 B15:C1001">
+  <conditionalFormatting sqref="I14:I1000 O14:O1000 B14:C1000 B1:C12 O1:O12 I1:I12">
     <cfRule type="expression" dxfId="170" priority="2" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D13 F1:F13 F15:F1001 B15:D1001">
+  <conditionalFormatting sqref="F14:F1000 B14:D1000 B1:D12 F1:F12">
     <cfRule type="expression" dxfId="169" priority="3" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D13 G1:H13 G15:H1001 B15:D1001">
+  <conditionalFormatting sqref="G14:H1000 B14:D1000 B1:D12 G1:H12">
     <cfRule type="expression" dxfId="168" priority="4" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D13 G1:H13 G15:H1001 B15:D1001">
+  <conditionalFormatting sqref="G14:H1000 B14:D1000 B1:D12 G1:H12">
     <cfRule type="expression" dxfId="167" priority="5" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C13 F1:F13 F15:F1001 B15:C1001">
+  <conditionalFormatting sqref="F14:F1000 B14:C1000 B1:C12 F1:F12">
     <cfRule type="expression" dxfId="166" priority="6" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F13 B1:B13 B15:B1001 F15:F1001">
+  <conditionalFormatting sqref="B14:B1000 F14:F1000 F1:F12 B1:B12">
     <cfRule type="expression" dxfId="165" priority="7" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C13 B15:C1001">
+  <conditionalFormatting sqref="B14:C1000 B1:C12">
     <cfRule type="expression" dxfId="164" priority="8" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C13 B15:C1001">
+  <conditionalFormatting sqref="B14:C1000 B1:C12">
     <cfRule type="expression" dxfId="163" priority="9" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C13 B15:C1001">
+  <conditionalFormatting sqref="B14:C1000 B1:C12">
     <cfRule type="expression" dxfId="162" priority="10" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N13 B1:B13 B15:B1001 N15:N1001">
+  <conditionalFormatting sqref="B14:B1000 N14:N1000 N1:N12 B1:B12">
     <cfRule type="expression" dxfId="161" priority="11" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C13 F1:F13 F15:F1001 B15:C1001">
+  <conditionalFormatting sqref="F14:F1000 B14:C1000 B1:C12 F1:F12">
     <cfRule type="expression" dxfId="160" priority="12" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C13 F1:F13 F15:F1001 B15:C1001">
+  <conditionalFormatting sqref="F14:F1000 B14:C1000 B1:C12 F1:F12">
     <cfRule type="expression" dxfId="159" priority="13" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C13 B15:C1001">
+  <conditionalFormatting sqref="B14:C1000 B1:C12">
     <cfRule type="expression" dxfId="158" priority="14" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="157" priority="15" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="156" priority="16" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="155" priority="17" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="154" priority="18" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="153" priority="19" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="152" priority="20" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="151" priority="21" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="150" priority="22" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="149" priority="23" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="148" priority="24" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="147" priority="25" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="146" priority="26" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="145" priority="27" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="144" priority="28" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="143" priority="29" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="142" priority="30" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="141" priority="31" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="140" priority="32" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W13 A15:W1001">
+  <conditionalFormatting sqref="A14:W1000 A1:W12">
     <cfRule type="expression" dxfId="139" priority="33" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B13 B15:B1001">
+  <conditionalFormatting sqref="B14:B1000 B1:B12">
     <cfRule type="expression" dxfId="138" priority="34" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B13 F1:F13 F15:F1001 B15:B1001">
+  <conditionalFormatting sqref="F14:F1000 B14:B1000 B1:B12 F1:F12">
     <cfRule type="expression" dxfId="137" priority="35" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="expression" dxfId="136" priority="36" stopIfTrue="1">
+      <formula>$A12="integer"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="expression" dxfId="135" priority="37" stopIfTrue="1">
+      <formula>$A12="decimal"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13 I13 F13">
+    <cfRule type="expression" dxfId="134" priority="38" stopIfTrue="1">
+      <formula>$A13="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13 O13 I13">
+    <cfRule type="expression" dxfId="133" priority="39" stopIfTrue="1">
+      <formula>$A13="begin repeat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:D13 F13">
+    <cfRule type="expression" dxfId="132" priority="40" stopIfTrue="1">
+      <formula>$A13="text"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:D13 G13:H13">
+    <cfRule type="expression" dxfId="131" priority="41" stopIfTrue="1">
+      <formula>$A13="integer"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:D13 G13:H13">
+    <cfRule type="expression" dxfId="130" priority="42" stopIfTrue="1">
+      <formula>$A13="decimal"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13 F13">
+    <cfRule type="expression" dxfId="129" priority="43" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A13, 16)="select_multiple ", LEN($A13)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A13, 17)))), AND(LEFT($A13, 11)="select_one ", LEN($A13)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A13, 12)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13 B13">
+    <cfRule type="expression" dxfId="128" priority="44" stopIfTrue="1">
+      <formula>OR($A13="audio audit", $A13="text audit", $A13="speed violations count", $A13="speed violations list", $A13="speed violations audit")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13">
+    <cfRule type="expression" dxfId="127" priority="45" stopIfTrue="1">
+      <formula>$A13="note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13">
+    <cfRule type="expression" dxfId="126" priority="46" stopIfTrue="1">
+      <formula>$A13="barcode"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13">
+    <cfRule type="expression" dxfId="125" priority="47" stopIfTrue="1">
+      <formula>OR($A13="geopoint", $A13="geoshape", $A13="geotrace")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N13 B13">
+    <cfRule type="expression" dxfId="124" priority="48" stopIfTrue="1">
+      <formula>OR($A13="calculate", $A13="calculate_here")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13 F13">
+    <cfRule type="expression" dxfId="123" priority="49" stopIfTrue="1">
+      <formula>OR($A13="date", $A13="datetime")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13 F13">
+    <cfRule type="expression" dxfId="122" priority="50" stopIfTrue="1">
+      <formula>$A13="image"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:C13">
+    <cfRule type="expression" dxfId="121" priority="51" stopIfTrue="1">
+      <formula>OR($A13="audio", $A13="video")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="120" priority="52" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A13, 14)="sensor_stream ", LEN($A13)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A13, 15)))), AND(LEFT($A13, 17)="sensor_statistic ", LEN($A13)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A13, 18)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="119" priority="53" stopIfTrue="1">
+      <formula>$A13="comments"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="118" priority="54" stopIfTrue="1">
+      <formula>OR($A13="audio", $A13="video")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="117" priority="55" stopIfTrue="1">
+      <formula>$A13="image"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="116" priority="56" stopIfTrue="1">
+      <formula>OR($A13="date", $A13="datetime")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="115" priority="57" stopIfTrue="1">
+      <formula>OR($A13="calculate", $A13="calculate_here")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="114" priority="58" stopIfTrue="1">
+      <formula>$A13="note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="113" priority="59" stopIfTrue="1">
+      <formula>$A13="barcode"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="112" priority="60" stopIfTrue="1">
+      <formula>OR($A13="geopoint", $A13="geoshape", $A13="geotrace")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="111" priority="61" stopIfTrue="1">
+      <formula>OR($A13="audio audit", $A13="text audit", $A13="speed violations count", $A13="speed violations list", $A13="speed violations audit")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="110" priority="62" stopIfTrue="1">
+      <formula>OR($A13="username", $A13="phonenumber", $A13="start", $A13="end", $A13="deviceid", $A13="subscriberid", $A13="simserial", $A13="caseid")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="109" priority="63" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A13, 16)="select_multiple ", LEN($A13)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A13, 17)))), AND(LEFT($A13, 11)="select_one ", LEN($A13)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A13, 12)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="108" priority="64" stopIfTrue="1">
+      <formula>$A13="decimal"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="107" priority="65" stopIfTrue="1">
+      <formula>$A13="integer"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="106" priority="66" stopIfTrue="1">
+      <formula>$A13="text"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="105" priority="67" stopIfTrue="1">
+      <formula>$A13="end repeat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="104" priority="68" stopIfTrue="1">
+      <formula>$A13="begin repeat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="103" priority="69" stopIfTrue="1">
+      <formula>$A13="end group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:W13">
+    <cfRule type="expression" dxfId="102" priority="70" stopIfTrue="1">
+      <formula>$A13="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="expression" dxfId="101" priority="71" stopIfTrue="1">
+      <formula>$A13="comments"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13 F13">
+    <cfRule type="expression" dxfId="100" priority="72" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A13, 14)="sensor_stream ", LEN($A13)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A13, 15)))), AND(LEFT($A13, 17)="sensor_statistic ", LEN($A13)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A13, 18)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="136" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="73" stopIfTrue="1">
       <formula>$A13="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="135" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="74" stopIfTrue="1">
       <formula>$A13="decimal"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C14 I14 F14">
-    <cfRule type="expression" dxfId="134" priority="38" stopIfTrue="1">
-      <formula>$A14="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C14 O14 I14">
-    <cfRule type="expression" dxfId="133" priority="39" stopIfTrue="1">
-      <formula>$A14="begin repeat"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:D14 F14">
-    <cfRule type="expression" dxfId="132" priority="40" stopIfTrue="1">
-      <formula>$A14="text"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:D14 G14:H14">
-    <cfRule type="expression" dxfId="131" priority="41" stopIfTrue="1">
-      <formula>$A14="integer"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:D14 G14:H14">
-    <cfRule type="expression" dxfId="130" priority="42" stopIfTrue="1">
-      <formula>$A14="decimal"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C14 F14">
-    <cfRule type="expression" dxfId="129" priority="43" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A14, 16)="select_multiple ", LEN($A14)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A14, 17)))), AND(LEFT($A14, 11)="select_one ", LEN($A14)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A14, 12)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F14 B14">
-    <cfRule type="expression" dxfId="128" priority="44" stopIfTrue="1">
-      <formula>OR($A14="audio audit", $A14="text audit", $A14="speed violations count", $A14="speed violations list", $A14="speed violations audit")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C14">
-    <cfRule type="expression" dxfId="127" priority="45" stopIfTrue="1">
-      <formula>$A14="note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C14">
-    <cfRule type="expression" dxfId="126" priority="46" stopIfTrue="1">
-      <formula>$A14="barcode"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C14">
-    <cfRule type="expression" dxfId="125" priority="47" stopIfTrue="1">
-      <formula>OR($A14="geopoint", $A14="geoshape", $A14="geotrace")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N14 B14">
-    <cfRule type="expression" dxfId="124" priority="48" stopIfTrue="1">
-      <formula>OR($A14="calculate", $A14="calculate_here")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C14 F14">
-    <cfRule type="expression" dxfId="123" priority="49" stopIfTrue="1">
-      <formula>OR($A14="date", $A14="datetime")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C14 F14">
-    <cfRule type="expression" dxfId="122" priority="50" stopIfTrue="1">
-      <formula>$A14="image"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:C14">
-    <cfRule type="expression" dxfId="121" priority="51" stopIfTrue="1">
-      <formula>OR($A14="audio", $A14="video")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="120" priority="52" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A14, 14)="sensor_stream ", LEN($A14)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A14, 15)))), AND(LEFT($A14, 17)="sensor_statistic ", LEN($A14)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A14, 18)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="119" priority="53" stopIfTrue="1">
-      <formula>$A14="comments"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="118" priority="54" stopIfTrue="1">
-      <formula>OR($A14="audio", $A14="video")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="117" priority="55" stopIfTrue="1">
-      <formula>$A14="image"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="116" priority="56" stopIfTrue="1">
-      <formula>OR($A14="date", $A14="datetime")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="115" priority="57" stopIfTrue="1">
-      <formula>OR($A14="calculate", $A14="calculate_here")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="114" priority="58" stopIfTrue="1">
-      <formula>$A14="note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="113" priority="59" stopIfTrue="1">
-      <formula>$A14="barcode"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="112" priority="60" stopIfTrue="1">
-      <formula>OR($A14="geopoint", $A14="geoshape", $A14="geotrace")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="111" priority="61" stopIfTrue="1">
-      <formula>OR($A14="audio audit", $A14="text audit", $A14="speed violations count", $A14="speed violations list", $A14="speed violations audit")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="110" priority="62" stopIfTrue="1">
-      <formula>OR($A14="username", $A14="phonenumber", $A14="start", $A14="end", $A14="deviceid", $A14="subscriberid", $A14="simserial", $A14="caseid")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="109" priority="63" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A14, 16)="select_multiple ", LEN($A14)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A14, 17)))), AND(LEFT($A14, 11)="select_one ", LEN($A14)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A14, 12)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="108" priority="64" stopIfTrue="1">
-      <formula>$A14="decimal"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="107" priority="65" stopIfTrue="1">
-      <formula>$A14="integer"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="106" priority="66" stopIfTrue="1">
-      <formula>$A14="text"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="105" priority="67" stopIfTrue="1">
-      <formula>$A14="end repeat"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="104" priority="68" stopIfTrue="1">
-      <formula>$A14="begin repeat"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="103" priority="69" stopIfTrue="1">
-      <formula>$A14="end group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:W14">
-    <cfRule type="expression" dxfId="102" priority="70" stopIfTrue="1">
-      <formula>$A14="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="101" priority="71" stopIfTrue="1">
-      <formula>$A14="comments"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14 F14">
-    <cfRule type="expression" dxfId="100" priority="72" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A14, 14)="sensor_stream ", LEN($A14)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A14, 15)))), AND(LEFT($A14, 17)="sensor_statistic ", LEN($A14)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A14, 18)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F14">
-    <cfRule type="expression" dxfId="99" priority="73" stopIfTrue="1">
-      <formula>$A14="integer"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F14">
-    <cfRule type="expression" dxfId="98" priority="74" stopIfTrue="1">
-      <formula>$A14="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0" footer="0"/>
@@ -18955,7 +18927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -19011,14 +18983,14 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C2" s="12" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2103051607</v>
+        <v>2103051617</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>58</v>

</xml_diff>